<commit_message>
3D Print Error bar post
</commit_message>
<xml_diff>
--- a/content/code/matplotlib_plots/3D-printed_tensile_test_data.xlsx
+++ b/content/code/matplotlib_plots/3D-printed_tensile_test_data.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="8">
   <si>
-    <t xml:space="preserve">Label</t>
+    <t xml:space="preserve">Material</t>
   </si>
   <si>
     <t xml:space="preserve">Width (mm)</t>
@@ -40,51 +40,26 @@
     <t xml:space="preserve">Tensile Strength (Mpa)</t>
   </si>
   <si>
-    <t xml:space="preserve">1 black</t>
+    <t xml:space="preserve">ABS</t>
   </si>
   <si>
-    <t xml:space="preserve">2 light blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 dark blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 dark blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
+    <t xml:space="preserve">HIPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,9 +119,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -166,20 +153,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,7 +213,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>6.27</v>
@@ -248,7 +235,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>6.29</v>
@@ -270,7 +257,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>6.28</v>
@@ -292,7 +279,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6.25</v>
@@ -314,7 +301,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6.26</v>
@@ -335,8 +322,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
+      <c r="A8" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6.29</v>
@@ -357,8 +344,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>2</v>
+      <c r="A9" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6.3</v>
@@ -379,8 +366,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>3</v>
+      <c r="A10" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6.34</v>
@@ -401,8 +388,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>4</v>
+      <c r="A11" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>6.2</v>
@@ -423,13 +410,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>5</v>
+      <c r="A12" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>6.28</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>3.62</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -446,12 +433,12 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>6.45</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>3.59</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -468,12 +455,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>6.29</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>3.57</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -490,12 +477,12 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>6.25</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>3.61</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -512,12 +499,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>6.29</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>3.58</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -534,12 +521,12 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>6.4</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>3.61</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -552,6 +539,446 @@
       <c r="F17" s="0" t="n">
         <f aca="false">E17/D17</f>
         <v>19.5204293628809</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">B18*C18</f>
+        <v>23.125</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>240</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">E18/D18</f>
+        <v>10.3783783783784</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>6.27</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>6.63</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">B19*C19</f>
+        <v>41.5701</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>205</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">E19/D19</f>
+        <v>4.93142908003589</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">B20*C20</f>
+        <v>23.712</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>243</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">E20/D20</f>
+        <v>10.247975708502</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">B21*C21</f>
+        <v>22.922</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>240</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <f aca="false">E21/D21</f>
+        <v>10.4702905505628</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">B22*C22</f>
+        <v>22.8956</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>249</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">E22/D22</f>
+        <v>10.8754520519226</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">B23*C23</f>
+        <v>22.63</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>291</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">E23/D23</f>
+        <v>12.8590366769775</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">B24*C24</f>
+        <v>23.312</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>276</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false">E24/D24</f>
+        <v>11.8393960192176</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>6.24</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">B25*C25</f>
+        <v>23.712</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">E25/D25</f>
+        <v>8.43454790823212</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">B26*C26</f>
+        <v>23.236</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <f aca="false">E26/D26</f>
+        <v>9.98450679979342</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">B27*C27</f>
+        <v>22.8125</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>241</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <f aca="false">E27/D27</f>
+        <v>10.5643835616438</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">B28*C28</f>
+        <v>24.3514</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <f aca="false">E28/D28</f>
+        <v>8.58266875826441</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">B29*C29</f>
+        <v>22.7173</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>221</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <f aca="false">E29/D29</f>
+        <v>9.72826876433379</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">B30*C30</f>
+        <v>22.7173</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>245</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <f aca="false">E30/D30</f>
+        <v>10.784732340551</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">B31*C31</f>
+        <v>22.8125</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>245</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <f aca="false">E31/D31</f>
+        <v>10.7397260273973</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">B32*C32</f>
+        <v>22.63</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>248</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <f aca="false">E32/D32</f>
+        <v>10.958904109589</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">B33*C33</f>
+        <v>22.7173</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>282</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <f aca="false">E33/D33</f>
+        <v>12.4134470205526</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>6.28</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">B34*C34</f>
+        <v>22.922</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>306</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <f aca="false">E34/D34</f>
+        <v>13.3496204519675</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">B35*C35</f>
+        <v>22.8956</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>260</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <f aca="false">E35/D35</f>
+        <v>11.3558937088349</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">B36*C36</f>
+        <v>22.63</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>334</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <f aca="false">E36/D36</f>
+        <v>14.7591692443659</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">B37*C37</f>
+        <v>23.125</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>312</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <f aca="false">E37/D37</f>
+        <v>13.4918918918919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>